<commit_message>
predicting on probability now
</commit_message>
<xml_diff>
--- a/RankingResults.xlsx
+++ b/RankingResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Documents\GitHub\Machine-Learning-Poly-U\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F299E3-E3FE-4C32-A9DC-5489B813686F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DE48D3-84DC-4550-B615-313227F68C20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="3396" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{CA10C3E9-C0E7-48B3-A698-9B6D501A1E63}"/>
+    <workbookView xWindow="14244" yWindow="1908" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{CA10C3E9-C0E7-48B3-A698-9B6D501A1E63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>Linear Regression</t>
   </si>
@@ -75,15 +75,25 @@
   <si>
     <t>Random Forest</t>
   </si>
+  <si>
+    <t>Lasso Regression</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -109,10 +119,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -587,53 +598,59 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$A$2:$A$7</c:f>
+              <c:f>Sheet2!$A$2:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>Logistic Regression</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Neural Network MLP Classification</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Lasso Regression</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>K Nearest Neighbors</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>Support Vector Classification</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>Support Vector Regression</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>Naïve Bayes GaussianNB</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Neural Network MLP Classification</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$2:$B$7</c:f>
+              <c:f>Sheet2!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.76</c:v>
+                  <c:v>0.84199999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.84199999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.76129999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.69330000000000003</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0%">
+                <c:pt idx="4" formatCode="0%">
                   <c:v>0.68</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="0%">
+                <c:pt idx="5" formatCode="0%">
                   <c:v>0.68</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="0%">
+                <c:pt idx="6" formatCode="0%">
                   <c:v>0.64</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="0%">
-                  <c:v>0.76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2408,10 +2425,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17906E50-2767-481A-B13C-BE3CD2FC2396}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2432,51 +2449,63 @@
         <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>0.76</v>
+        <v>0.84199999999999997</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2">
-        <v>0.69330000000000003</v>
+        <v>0.84199999999999997</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0.68</v>
+        <v>14</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.76129999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0.68</v>
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.69330000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>7</v>
+      <c r="A6" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>0.64</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>6</v>
+      <c r="A7" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="B7" s="1">
-        <v>0.76</v>
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.64</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B7">
+    <sortCondition descending="1" ref="B1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update to code, simplified, update to ppt
</commit_message>
<xml_diff>
--- a/RankingResults.xlsx
+++ b/RankingResults.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Documents\GitHub\Machine-Learning-Poly-U\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EDEF9EC-D2DE-462A-88A0-453A385AFAA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A2CB2E-D5B0-4748-A8AE-D66F4704C006}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CA10C3E9-C0E7-48B3-A698-9B6D501A1E63}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{CA10C3E9-C0E7-48B3-A698-9B6D501A1E63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$B$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet3!$A$1:$B$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
   <si>
     <t>Linear Regression</t>
   </si>
@@ -80,6 +82,9 @@
   </si>
   <si>
     <t>Lasso Regression</t>
+  </si>
+  <si>
+    <t>Combination</t>
   </si>
 </sst>
 </file>
@@ -605,13 +610,13 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>Lasso Regression</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Logistic Regression</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>Neural Network MLP Classification</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Lasso Regression</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>K Nearest Neighbors</c:v>
@@ -635,13 +640,13 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.76129999999999998</c:v>
+                  <c:v>0.77129999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.76129999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.76129999999999998</c:v>
+                  <c:v>0.74129999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.69330000000000003</c:v>
@@ -836,6 +841,300 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Score</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Lasso Regression</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Logistic Regression</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Combination</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Neural Network MLP Classification</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.84699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.84199999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.83799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.80500000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3684-42D2-8560-79014FA87764}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1821458752"/>
+        <c:axId val="1819502288"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1821458752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1819502288"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1819502288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1821458752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -916,6 +1215,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1420,6 +1759,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1984,6 +2826,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7E1DA0E-C993-498E-AA69-5469A34DBB5E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1135380</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{415B96AB-C4C7-45EE-AE34-3F6275EF6898}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2303,7 +3186,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EF75C46-3F11-45B6-97FE-7AB67440E6B1}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -2431,8 +3314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17906E50-2767-481A-B13C-BE3CD2FC2396}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2450,15 +3333,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2">
-        <v>0.76129999999999998</v>
+        <v>0.77129999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2">
         <v>0.76129999999999998</v>
@@ -2466,10 +3349,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2">
-        <v>0.76129999999999998</v>
+        <v>0.74129999999999996</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2505,11 +3388,73 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B7">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B8">
     <sortCondition descending="1" ref="B1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F71907F0-ADBB-4EE6-A971-C38BDB985002}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.84699999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.84199999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.83799999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.80500000000000005</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B5">
+    <sortCondition descending="1" ref="B1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updates to code and ppt
</commit_message>
<xml_diff>
--- a/RankingResults.xlsx
+++ b/RankingResults.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Documents\GitHub\Machine-Learning-Poly-U\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A2CB2E-D5B0-4748-A8AE-D66F4704C006}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD19083-03DD-44D6-B5F7-F6C30BB84E05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{CA10C3E9-C0E7-48B3-A698-9B6D501A1E63}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{CA10C3E9-C0E7-48B3-A698-9B6D501A1E63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$B$13</definedName>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
   <si>
     <t>Linear Regression</t>
   </si>
@@ -1135,6 +1136,294 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet4!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Score</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet4!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Logistic Regression</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Neural Network MLP Classification</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Lasso Regression</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.76300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.72699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.70599999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BA72-454E-9DF9-0C6A7B46A22D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1727077360"/>
+        <c:axId val="1634035584"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1727077360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1634035584"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1634035584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1727077360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1255,6 +1544,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2262,6 +2591,509 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2867,6 +3699,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{415B96AB-C4C7-45EE-AE34-3F6275EF6898}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>259080</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1317FF5D-38F5-4D8B-BB93-E68810449B46}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3314,7 +4187,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17906E50-2767-481A-B13C-BE3CD2FC2396}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
@@ -3402,7 +4275,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3457,4 +4330,55 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9AC816-10DA-4ABC-B1B0-9B0E4319DDA1}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.76300000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.72699999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.70599999999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B4">
+    <sortCondition descending="1" ref="B1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>